<commit_message>
20201030 INT20-0042	Fix eHSU0006 Report 20201105 INT20-0045	Fix display of LAIV in last 3 vaccine column in VF001 report 20201108 CRE20-015	HA Scheme 20201108 CRE20-014	To add new seasonal influenza vaccine under VSS and PPP-KG with subsidy at $100 per dose 20201108 INT20-0037	Fix deadlock on claim creation 20201108 INT20-0043	Fix error when change Doc Type on HCVU Vaccination File Rectification 20201108 INT20-0044	Fix batch upload with invalid DOB 20201109 INT20-0046	Change Gov SIV claim start date 20201110 INT20-0048	Fix no response on 2nd Authorization scheme click 20201110 INT20-0047	Fix exception on edit account with invalid CCCode
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSD0028-VSS Claim_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSD0028-VSS Claim_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019\EHS\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019_BatchUpload\ExcelGenerator\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,12 +20,12 @@
     <sheet name="Remark" sheetId="6" r:id="rId6"/>
     <sheet name="Change History" sheetId="25" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="144">
   <si>
     <t/>
   </si>
@@ -540,11 +540,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -687,7 +687,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -699,13 +699,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -723,22 +723,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -747,22 +747,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -774,7 +774,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -822,7 +822,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -987,7 +987,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,7 +1059,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1929,13 +1929,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF75"/>
+  <dimension ref="A1:AF84"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="18.625" style="71"/>
+    <col min="1" max="1" width="22.625" style="71" customWidth="1"/>
+    <col min="2" max="16" width="18.625" style="71"/>
     <col min="17" max="19" width="18.625" style="140"/>
     <col min="20" max="16384" width="18.625" style="71"/>
   </cols>
@@ -2632,7 +2633,7 @@
       <c r="AE43" s="78"/>
     </row>
     <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="114" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="26" t="s">
@@ -2722,7 +2723,7 @@
       <c r="AF44" s="26"/>
     </row>
     <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="71" t="s">
+      <c r="A45" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="26" t="s">
@@ -2812,7 +2813,7 @@
       <c r="AF45" s="26"/>
     </row>
     <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="59" t="s">
+      <c r="A46" s="114" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="26" t="s">
@@ -2902,7 +2903,7 @@
       <c r="AF46" s="26"/>
     </row>
     <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="71" t="s">
+      <c r="A47" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="26" t="s">
@@ -2992,7 +2993,7 @@
       <c r="AF47" s="26"/>
     </row>
     <row r="48" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="59" t="s">
+      <c r="A48" s="114" t="s">
         <v>26</v>
       </c>
       <c r="B48" s="130" t="s">
@@ -3082,7 +3083,7 @@
       <c r="AF48" s="130"/>
     </row>
     <row r="49" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="140" t="s">
+      <c r="A49" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="130" t="s">
@@ -3172,7 +3173,7 @@
       <c r="AF49" s="130"/>
     </row>
     <row r="50" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="59" t="s">
+      <c r="A50" s="114" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="26" t="s">
@@ -3262,7 +3263,7 @@
       <c r="AF50" s="26"/>
     </row>
     <row r="51" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="26" t="s">
@@ -3352,7 +3353,7 @@
       <c r="AF51" s="26"/>
     </row>
     <row r="52" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="114" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="26" t="s">
@@ -3442,7 +3443,7 @@
       <c r="AF52" s="26"/>
     </row>
     <row r="53" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="71" t="s">
+      <c r="A53" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="26" t="s">
@@ -3532,7 +3533,7 @@
       <c r="AF53" s="26"/>
     </row>
     <row r="54" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="26" t="s">
@@ -3622,7 +3623,7 @@
       <c r="AF54" s="26"/>
     </row>
     <row r="55" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="140" t="s">
+      <c r="A55" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B55" s="130" t="s">
@@ -3712,7 +3713,7 @@
       <c r="AF55" s="130"/>
     </row>
     <row r="56" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="140" t="s">
+      <c r="A56" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B56" s="130" t="s">
@@ -3802,7 +3803,7 @@
       <c r="AF56" s="130"/>
     </row>
     <row r="57" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="140" t="s">
+      <c r="A57" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="130" t="s">
@@ -3891,390 +3892,503 @@
       <c r="AE57" s="130"/>
       <c r="AF57" s="130"/>
     </row>
-    <row r="58" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="I58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="J58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="K58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="L58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="M58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="N58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="O58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="P58" s="26" t="s">
-        <v>42</v>
+    <row r="58" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P58" s="130" t="s">
+        <v>26</v>
       </c>
       <c r="Q58" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="R58" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S58" s="130" t="s">
-        <v>42</v>
-      </c>
-      <c r="T58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="U58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="V58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="W58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="X58" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y58" s="26" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="T58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X58" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y58" s="130" t="s">
+        <v>26</v>
       </c>
       <c r="Z58" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AA58" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AB58" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AC58" s="130"/>
       <c r="AD58" s="130"/>
-      <c r="AE58" s="26"/>
-      <c r="AF58" s="26"/>
-    </row>
-    <row r="59" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="26"/>
-      <c r="O59" s="26"/>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="130"/>
-      <c r="R59" s="130"/>
-      <c r="S59" s="130"/>
-      <c r="T59" s="26"/>
-      <c r="U59" s="26"/>
-      <c r="V59" s="26"/>
-      <c r="W59" s="26"/>
-      <c r="X59" s="26"/>
-      <c r="Y59" s="26"/>
-      <c r="Z59" s="130"/>
-      <c r="AA59" s="130"/>
-      <c r="AB59" s="130"/>
+      <c r="AE58" s="130"/>
+      <c r="AF58" s="130"/>
+    </row>
+    <row r="59" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA59" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB59" s="130" t="s">
+        <v>26</v>
+      </c>
       <c r="AC59" s="130"/>
       <c r="AD59" s="130"/>
-      <c r="AE59" s="26"/>
-      <c r="AF59" s="26"/>
-    </row>
-    <row r="60" spans="1:32" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="116" t="s">
-        <v>131</v>
-      </c>
-      <c r="B60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="E60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="G60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="H60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="I60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="J60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="K60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="L60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="M60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="N60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="O60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="P60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="R60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="S60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="T60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="U60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="V60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="W60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="X60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB60" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC60" s="90"/>
-      <c r="AD60" s="90"/>
-      <c r="AE60" s="90"/>
-      <c r="AF60" s="90"/>
-    </row>
-    <row r="61" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="26"/>
-      <c r="O61" s="26"/>
-      <c r="P61" s="26"/>
-      <c r="Q61" s="130"/>
-      <c r="R61" s="130"/>
-      <c r="S61" s="130"/>
-      <c r="T61" s="26"/>
-      <c r="U61" s="26"/>
-      <c r="V61" s="26"/>
-      <c r="W61" s="26"/>
-      <c r="X61" s="26"/>
-      <c r="Y61" s="26"/>
-      <c r="Z61" s="130"/>
-      <c r="AA61" s="130"/>
-      <c r="AB61" s="130"/>
+      <c r="AE59" s="130"/>
+      <c r="AF59" s="130"/>
+    </row>
+    <row r="60" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB60" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC60" s="130"/>
+      <c r="AD60" s="130"/>
+      <c r="AE60" s="130"/>
+      <c r="AF60" s="130"/>
+    </row>
+    <row r="61" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="J61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="L61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="M61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="N61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="O61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="P61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="R61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="S61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="T61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="U61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="V61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="W61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="X61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA61" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB61" s="130" t="s">
+        <v>27</v>
+      </c>
       <c r="AC61" s="130"/>
       <c r="AD61" s="130"/>
-      <c r="AE61" s="26"/>
-      <c r="AF61" s="26"/>
-    </row>
-    <row r="62" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="I62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="J62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="K62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="L62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="M62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="N62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="O62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="P62" s="26" t="s">
-        <v>42</v>
+      <c r="AE61" s="130"/>
+      <c r="AF61" s="130"/>
+    </row>
+    <row r="62" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P62" s="130" t="s">
+        <v>26</v>
       </c>
       <c r="Q62" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="R62" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="S62" s="130" t="s">
-        <v>42</v>
-      </c>
-      <c r="T62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="U62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="V62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="W62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="X62" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y62" s="26" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="T62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X62" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y62" s="130" t="s">
+        <v>26</v>
       </c>
       <c r="Z62" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AA62" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AB62" s="130" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="AC62" s="130"/>
       <c r="AD62" s="130"/>
-      <c r="AE62" s="26"/>
-      <c r="AF62" s="26"/>
-    </row>
-    <row r="63" spans="1:32" s="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="103" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="G63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="H63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="I63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="J63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="K63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="L63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="M63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="N63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="O63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="P63" s="105" t="s">
+      <c r="AE62" s="130"/>
+      <c r="AF62" s="130"/>
+    </row>
+    <row r="63" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P63" s="130" t="s">
         <v>26</v>
       </c>
       <c r="Q63" s="130" t="s">
@@ -4286,22 +4400,22 @@
       <c r="S63" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="T63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="U63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="V63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="W63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="X63" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y63" s="105" t="s">
+      <c r="T63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X63" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y63" s="130" t="s">
         <v>26</v>
       </c>
       <c r="Z63" s="130" t="s">
@@ -4315,146 +4429,146 @@
       </c>
       <c r="AC63" s="130"/>
       <c r="AD63" s="130"/>
-      <c r="AE63" s="105"/>
-      <c r="AF63" s="105"/>
-    </row>
-    <row r="64" spans="1:32" s="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="103" t="s">
-        <v>83</v>
-      </c>
-      <c r="B64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="D64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="E64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="F64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="G64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="H64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="I64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="J64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="K64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="L64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="M64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="N64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="O64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="P64" s="105" t="s">
-        <v>26</v>
+      <c r="AE63" s="130"/>
+      <c r="AF63" s="130"/>
+    </row>
+    <row r="64" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="J64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="L64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="M64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="N64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="O64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="P64" s="130" t="s">
+        <v>27</v>
       </c>
       <c r="Q64" s="130" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R64" s="130" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S64" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="T64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="U64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="V64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="W64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="X64" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y64" s="105" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="T64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="U64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="V64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="W64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="X64" s="130" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y64" s="130" t="s">
+        <v>27</v>
       </c>
       <c r="Z64" s="130" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AA64" s="130" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB64" s="130" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC64" s="130"/>
       <c r="AD64" s="130"/>
-      <c r="AE64" s="105"/>
-      <c r="AF64" s="105"/>
-    </row>
-    <row r="65" spans="1:32" s="94" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="D65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="H65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="I65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="J65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="K65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="L65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="M65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="N65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="O65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="P65" s="105" t="s">
+      <c r="AE64" s="130"/>
+      <c r="AF64" s="130"/>
+    </row>
+    <row r="65" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P65" s="130" t="s">
         <v>26</v>
       </c>
       <c r="Q65" s="130" t="s">
@@ -4466,22 +4580,22 @@
       <c r="S65" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="T65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="U65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="V65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="W65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="X65" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y65" s="105" t="s">
+      <c r="T65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X65" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y65" s="130" t="s">
         <v>26</v>
       </c>
       <c r="Z65" s="130" t="s">
@@ -4495,12 +4609,12 @@
       </c>
       <c r="AC65" s="130"/>
       <c r="AD65" s="130"/>
-      <c r="AE65" s="105"/>
-      <c r="AF65" s="105"/>
-    </row>
-    <row r="66" spans="1:32" s="140" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="141" t="s">
-        <v>143</v>
+      <c r="AE65" s="130"/>
+      <c r="AF65" s="130"/>
+    </row>
+    <row r="66" spans="1:32" s="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
+        <v>26</v>
       </c>
       <c r="B66" s="130" t="s">
         <v>26</v>
@@ -4588,154 +4702,851 @@
       <c r="AE66" s="130"/>
       <c r="AF66" s="130"/>
     </row>
-    <row r="67" spans="1:32" s="140" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="141" t="s">
-        <v>142</v>
-      </c>
-      <c r="B67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="D67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="F67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="G67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="H67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="I67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="J67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="K67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="L67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="M67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="N67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="O67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="P67" s="130" t="s">
-        <v>26</v>
+    <row r="67" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="L67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="M67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="N67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="O67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P67" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="Q67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="R67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="S67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="T67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="U67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="V67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="W67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="X67" s="130" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="T67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="U67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="V67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="W67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="X67" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y67" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="Z67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AA67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AB67" s="130" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AC67" s="130"/>
       <c r="AD67" s="130"/>
-      <c r="AE67" s="130"/>
-      <c r="AF67" s="130"/>
-    </row>
-    <row r="68" spans="1:32" s="100" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F68" s="102"/>
-      <c r="G68" s="101"/>
-      <c r="Q68" s="140"/>
-      <c r="R68" s="140"/>
-      <c r="S68" s="140"/>
-    </row>
-    <row r="69" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
+      <c r="AE67" s="26"/>
+      <c r="AF67" s="26"/>
+    </row>
+    <row r="68" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="26"/>
+      <c r="N68" s="26"/>
+      <c r="O68" s="26"/>
+      <c r="P68" s="26"/>
+      <c r="Q68" s="130"/>
+      <c r="R68" s="130"/>
+      <c r="S68" s="130"/>
+      <c r="T68" s="26"/>
+      <c r="U68" s="26"/>
+      <c r="V68" s="26"/>
+      <c r="W68" s="26"/>
+      <c r="X68" s="26"/>
+      <c r="Y68" s="26"/>
+      <c r="Z68" s="130"/>
+      <c r="AA68" s="130"/>
+      <c r="AB68" s="130"/>
+      <c r="AC68" s="130"/>
+      <c r="AD68" s="130"/>
+      <c r="AE68" s="26"/>
+      <c r="AF68" s="26"/>
+    </row>
+    <row r="69" spans="1:32" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="116" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="F69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="G69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="H69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="I69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="J69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="K69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="L69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="M69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="N69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="O69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="P69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="R69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="S69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="T69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="U69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="V69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="W69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="X69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB69" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC69" s="90"/>
+      <c r="AD69" s="90"/>
+      <c r="AE69" s="90"/>
+      <c r="AF69" s="90"/>
     </row>
     <row r="70" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+      <c r="M70" s="26"/>
+      <c r="N70" s="26"/>
+      <c r="O70" s="26"/>
+      <c r="P70" s="26"/>
+      <c r="Q70" s="130"/>
+      <c r="R70" s="130"/>
+      <c r="S70" s="130"/>
+      <c r="T70" s="26"/>
+      <c r="U70" s="26"/>
+      <c r="V70" s="26"/>
+      <c r="W70" s="26"/>
+      <c r="X70" s="26"/>
+      <c r="Y70" s="26"/>
+      <c r="Z70" s="130"/>
+      <c r="AA70" s="130"/>
+      <c r="AB70" s="130"/>
+      <c r="AC70" s="130"/>
+      <c r="AD70" s="130"/>
+      <c r="AE70" s="26"/>
+      <c r="AF70" s="26"/>
     </row>
     <row r="71" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="L71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="M71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="N71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="O71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="R71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="S71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="T71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="U71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="V71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="W71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="X71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y71" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB71" s="130" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC71" s="130"/>
+      <c r="AD71" s="130"/>
+      <c r="AE71" s="26"/>
+      <c r="AF71" s="26"/>
+    </row>
+    <row r="72" spans="1:32" s="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="103" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="I72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="J72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="K72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="L72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="M72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="O72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="P72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="U72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="V72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="W72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="X72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y72" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB72" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC72" s="130"/>
+      <c r="AD72" s="130"/>
+      <c r="AE72" s="105"/>
+      <c r="AF72" s="105"/>
+    </row>
+    <row r="73" spans="1:32" s="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="103" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="I73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="J73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="K73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="L73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="M73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="O73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="P73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="U73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="V73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="W73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="X73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y73" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB73" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC73" s="130"/>
+      <c r="AD73" s="130"/>
+      <c r="AE73" s="105"/>
+      <c r="AF73" s="105"/>
+    </row>
+    <row r="74" spans="1:32" s="94" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="H74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="I74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="J74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="K74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="L74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="M74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="O74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="P74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="U74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="V74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="W74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="X74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y74" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB74" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC74" s="130"/>
+      <c r="AD74" s="130"/>
+      <c r="AE74" s="105"/>
+      <c r="AF74" s="105"/>
+    </row>
+    <row r="75" spans="1:32" s="140" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="141" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB75" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC75" s="130"/>
+      <c r="AD75" s="130"/>
+      <c r="AE75" s="130"/>
+      <c r="AF75" s="130"/>
+    </row>
+    <row r="76" spans="1:32" s="140" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="141" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="E76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="J76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="K76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="L76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="M76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="N76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="O76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="P76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="R76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="S76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="T76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="U76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="V76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="W76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="X76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB76" s="130" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC76" s="130"/>
+      <c r="AD76" s="130"/>
+      <c r="AE76" s="130"/>
+      <c r="AF76" s="130"/>
+    </row>
+    <row r="77" spans="1:32" s="100" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F77" s="102"/>
+      <c r="G77" s="101"/>
+      <c r="Q77" s="140"/>
+      <c r="R77" s="140"/>
+      <c r="S77" s="140"/>
+    </row>
+    <row r="78" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+    </row>
+    <row r="79" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" s="72"/>
+      <c r="C79" s="72"/>
+      <c r="D79" s="72"/>
+      <c r="E79" s="72"/>
+    </row>
+    <row r="80" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="106" t="s">
+    <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="106" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="106" t="s">
+    <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="77"/>
-      <c r="G73" s="77"/>
-    </row>
-    <row r="74" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="106" t="s">
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="77"/>
+      <c r="G82" s="77"/>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="106" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="106" t="s">
+    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="72"/>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
+      <c r="B84" s="72"/>
+      <c r="C84" s="72"/>
+      <c r="D84" s="72"/>
+      <c r="E84" s="72"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>